<commit_message>
created python notebook to produce csvs on election data in PA counties 2016
</commit_message>
<xml_diff>
--- a/proj_data/poverty_alldata.xlsx
+++ b/proj_data/poverty_alldata.xlsx
@@ -5848,8 +5848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7169,7 +7169,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>

</xml_diff>